<commit_message>
xml parser for greenbelt and olympic
</commit_message>
<xml_diff>
--- a/web/upload/green.xlsx
+++ b/web/upload/green.xlsx
@@ -13,15 +13,16 @@
     <sheet name="Sheet3" sheetId="3" state="visible" r:id="rId4"/>
   </sheets>
   <definedNames>
-    <definedName function="false" hidden="true" localSheetId="0" name="_xlnm._FilterDatabase" vbProcedure="false">Sheet1!$A$1:$I$12</definedName>
-    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase" vbProcedure="false">Sheet1!$A$1:$I$12</definedName>
+    <definedName function="false" hidden="true" localSheetId="0" name="_xlnm._FilterDatabase" vbProcedure="false">Sheet1!$A$1:$I$4</definedName>
+    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase" vbProcedure="false">Sheet1!$A$1:$I$4</definedName>
+    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase_0" vbProcedure="false">Sheet1!$A$1:$I$4</definedName>
   </definedNames>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.0001"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="61" uniqueCount="45">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="20">
   <si>
     <t>Rmt_No</t>
   </si>
@@ -75,81 +76,6 @@
   </si>
   <si>
     <t>Paid</t>
-  </si>
-  <si>
-    <t>SSC222589</t>
-  </si>
-  <si>
-    <t>MOHAMED MAHAMUD ALI</t>
-  </si>
-  <si>
-    <t>Nabila Ibrahim Isaaq</t>
-  </si>
-  <si>
-    <t>SSC222616</t>
-  </si>
-  <si>
-    <t>Abrehaley Seyoum Teklehaymanot</t>
-  </si>
-  <si>
-    <t>Barnebas Tsegay</t>
-  </si>
-  <si>
-    <t>SSC222618</t>
-  </si>
-  <si>
-    <t>Abdinasir Yusuf</t>
-  </si>
-  <si>
-    <t>Farxiya Maxamud Nur</t>
-  </si>
-  <si>
-    <t>SSC222630</t>
-  </si>
-  <si>
-    <t>Suad Saleban Omar</t>
-  </si>
-  <si>
-    <t>FAARAH KAARIYE FAARAH</t>
-  </si>
-  <si>
-    <t>STA222673</t>
-  </si>
-  <si>
-    <t>AMARIL_TAXES</t>
-  </si>
-  <si>
-    <t>DEEQA HASSAN AHMED</t>
-  </si>
-  <si>
-    <t>NASRA MOHAMED ALI</t>
-  </si>
-  <si>
-    <t>STA222680</t>
-  </si>
-  <si>
-    <t>HALIMA BEDEL ALI</t>
-  </si>
-  <si>
-    <t>ABDI BEDEL ALI</t>
-  </si>
-  <si>
-    <t>SSC222668</t>
-  </si>
-  <si>
-    <t>Abdirijak Ahmed Dahir</t>
-  </si>
-  <si>
-    <t>Nimo Adan Mohamoud</t>
-  </si>
-  <si>
-    <t>SSC222678</t>
-  </si>
-  <si>
-    <t>LUTFI OSMAN AHMED</t>
-  </si>
-  <si>
-    <t>Faadumo Mohamed Yusuf</t>
   </si>
   <si>
     <t>225 Records</t>
@@ -436,15 +362,15 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <sheetPr filterMode="false">
-    <tabColor rgb="00FFFFFF"/>
+    <tabColor rgb="FFFFFFFF"/>
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:I12"/>
+  <dimension ref="A1:I4"/>
   <sheetViews>
     <sheetView windowProtection="true" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <pane xSplit="0" ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="bottomLeft" activeCell="D14" activeCellId="0" sqref="D14"/>
+      <selection pane="bottomLeft" activeCell="C8" activeCellId="0" sqref="C8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
@@ -545,269 +471,29 @@
       </c>
     </row>
     <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="4" t="s">
+      <c r="A4" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="B4" s="5" t="s">
-        <v>10</v>
-      </c>
-      <c r="C4" s="5" t="s">
+      <c r="B4" s="14"/>
+      <c r="C4" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="D4" s="5" t="s">
-        <v>20</v>
-      </c>
-      <c r="E4" s="6" t="n">
-        <v>300</v>
-      </c>
-      <c r="F4" s="6" t="n">
-        <v>15</v>
-      </c>
-      <c r="G4" s="7" t="n">
-        <v>41995</v>
-      </c>
-      <c r="H4" s="7" t="n">
-        <v>42014</v>
-      </c>
-      <c r="I4" s="8" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="9" t="s">
-        <v>21</v>
-      </c>
-      <c r="B5" s="10" t="s">
-        <v>10</v>
-      </c>
-      <c r="C5" s="10" t="s">
-        <v>22</v>
-      </c>
-      <c r="D5" s="10" t="s">
-        <v>23</v>
-      </c>
-      <c r="E5" s="11" t="n">
-        <v>500</v>
-      </c>
-      <c r="F5" s="11" t="n">
-        <v>25</v>
-      </c>
-      <c r="G5" s="12" t="n">
-        <v>41996</v>
-      </c>
-      <c r="H5" s="12" t="n">
-        <v>42010</v>
-      </c>
-      <c r="I5" s="13" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="6" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="4" t="s">
-        <v>24</v>
-      </c>
-      <c r="B6" s="5" t="s">
-        <v>10</v>
-      </c>
-      <c r="C6" s="5" t="s">
-        <v>25</v>
-      </c>
-      <c r="D6" s="5" t="s">
-        <v>26</v>
-      </c>
-      <c r="E6" s="6" t="n">
-        <v>50</v>
-      </c>
-      <c r="F6" s="6" t="n">
-        <v>3</v>
-      </c>
-      <c r="G6" s="7" t="n">
-        <v>41996</v>
-      </c>
-      <c r="H6" s="7" t="n">
-        <v>42008</v>
-      </c>
-      <c r="I6" s="8" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="7" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="9" t="s">
-        <v>27</v>
-      </c>
-      <c r="B7" s="10" t="s">
-        <v>10</v>
-      </c>
-      <c r="C7" s="10" t="s">
-        <v>28</v>
-      </c>
-      <c r="D7" s="10" t="s">
-        <v>29</v>
-      </c>
-      <c r="E7" s="11" t="n">
-        <v>100</v>
-      </c>
-      <c r="F7" s="11" t="n">
-        <v>5</v>
-      </c>
-      <c r="G7" s="12" t="n">
-        <v>41996</v>
-      </c>
-      <c r="H7" s="12" t="n">
-        <v>42009</v>
-      </c>
-      <c r="I7" s="13" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="8" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="9" t="s">
-        <v>30</v>
-      </c>
-      <c r="B8" s="10" t="s">
-        <v>31</v>
-      </c>
-      <c r="C8" s="10" t="s">
-        <v>32</v>
-      </c>
-      <c r="D8" s="10" t="s">
-        <v>33</v>
-      </c>
-      <c r="E8" s="11" t="n">
-        <v>100</v>
-      </c>
-      <c r="F8" s="11" t="n">
-        <v>5</v>
-      </c>
-      <c r="G8" s="12" t="n">
-        <v>41997</v>
-      </c>
-      <c r="H8" s="12" t="n">
-        <v>42005</v>
-      </c>
-      <c r="I8" s="13" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="9" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A9" s="4" t="s">
-        <v>34</v>
-      </c>
-      <c r="B9" s="5" t="s">
-        <v>31</v>
-      </c>
-      <c r="C9" s="5" t="s">
-        <v>35</v>
-      </c>
-      <c r="D9" s="5" t="s">
-        <v>36</v>
-      </c>
-      <c r="E9" s="6" t="n">
-        <v>200</v>
-      </c>
-      <c r="F9" s="6" t="n">
-        <v>10</v>
-      </c>
-      <c r="G9" s="7" t="n">
-        <v>41997</v>
-      </c>
-      <c r="H9" s="7" t="n">
-        <v>42007</v>
-      </c>
-      <c r="I9" s="8" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="10" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A10" s="4" t="s">
-        <v>37</v>
-      </c>
-      <c r="B10" s="5" t="s">
-        <v>10</v>
-      </c>
-      <c r="C10" s="5" t="s">
-        <v>38</v>
-      </c>
-      <c r="D10" s="5" t="s">
-        <v>39</v>
-      </c>
-      <c r="E10" s="6" t="n">
-        <v>140</v>
-      </c>
-      <c r="F10" s="6" t="n">
-        <v>8</v>
-      </c>
-      <c r="G10" s="7" t="n">
-        <v>41997</v>
-      </c>
-      <c r="H10" s="7" t="n">
-        <v>42005</v>
-      </c>
-      <c r="I10" s="8" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="11" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A11" s="9" t="s">
-        <v>40</v>
-      </c>
-      <c r="B11" s="10" t="s">
-        <v>10</v>
-      </c>
-      <c r="C11" s="10" t="s">
-        <v>41</v>
-      </c>
-      <c r="D11" s="10" t="s">
-        <v>42</v>
-      </c>
-      <c r="E11" s="11" t="n">
-        <v>1000</v>
-      </c>
-      <c r="F11" s="11" t="n">
-        <v>40</v>
-      </c>
-      <c r="G11" s="12" t="n">
-        <v>41997</v>
-      </c>
-      <c r="H11" s="12" t="n">
-        <v>42009</v>
-      </c>
-      <c r="I11" s="13" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="12" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A12" s="1" t="s">
-        <v>43</v>
-      </c>
-      <c r="B12" s="14"/>
-      <c r="C12" s="1" t="s">
-        <v>44</v>
-      </c>
-      <c r="D12" s="14"/>
-      <c r="E12" s="15" t="n">
+      <c r="D4" s="14"/>
+      <c r="E4" s="15" t="n">
         <v>2264.5</v>
       </c>
-      <c r="F12" s="16" t="n">
+      <c r="F4" s="16" t="n">
         <v>48209.5</v>
       </c>
-      <c r="G12" s="17"/>
-      <c r="H12" s="17"/>
-      <c r="I12" s="17"/>
+      <c r="G4" s="17"/>
+      <c r="H4" s="17"/>
+      <c r="I4" s="17"/>
     </row>
   </sheetData>
-  <autoFilter ref="A1:I12"/>
+  <autoFilter ref="A1:I4"/>
   <hyperlinks>
     <hyperlink ref="A2" r:id="rId1" display="SSC222384"/>
     <hyperlink ref="A3" r:id="rId2" display="SSC222513"/>
-    <hyperlink ref="A4" r:id="rId3" display="SSC222589"/>
-    <hyperlink ref="A5" r:id="rId4" display="SSC222616"/>
-    <hyperlink ref="A6" r:id="rId5" display="SSC222618"/>
-    <hyperlink ref="A7" r:id="rId6" display="SSC222630"/>
-    <hyperlink ref="A8" r:id="rId7" display="STA222673"/>
-    <hyperlink ref="A9" r:id="rId8" display="STA222680"/>
-    <hyperlink ref="A10" r:id="rId9" display="SSC222668"/>
-    <hyperlink ref="A11" r:id="rId10" display="SSC222678"/>
   </hyperlinks>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
@@ -816,14 +502,14 @@
     <oddHeader/>
     <oddFooter/>
   </headerFooter>
-  <drawing r:id="rId11"/>
+  <drawing r:id="rId3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <sheetPr filterMode="false">
-    <tabColor rgb="00FFFFFF"/>
+    <tabColor rgb="FFFFFFFF"/>
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
   <dimension ref="A1"/>
@@ -850,7 +536,7 @@
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <sheetPr filterMode="false">
-    <tabColor rgb="00FFFFFF"/>
+    <tabColor rgb="FFFFFFFF"/>
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
   <dimension ref="A1"/>

</xml_diff>